<commit_message>
Added a new feature to the program. "Refresh prices"
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -400,7 +400,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>34365.63</v>
+        <v>30727.97</v>
       </c>
       <c r="C2" t="n">
         <v>500</v>
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2095.6</v>
+        <v>1820.37</v>
       </c>
       <c r="C3" t="n">
         <v>10</v>
@@ -489,6 +489,32 @@
       <c r="F3" t="inlineStr">
         <is>
           <t>05:29:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BNB</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>283.88</v>
+      </c>
+      <c r="C4" t="n">
+        <v>9</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2558.7</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>19/07/21</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>12:58:49</t>
         </is>
       </c>
     </row>

</xml_diff>